<commit_message>
Begin tfdif Parsing Reviews
</commit_message>
<xml_diff>
--- a/Data/Largest_Cities.xlsx
+++ b/Data/Largest_Cities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mariko\Documents\GitHub\Capstone-DATS6501\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B464385F-D815-4533-9B06-A65189821590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF46DBFB-A797-41AE-92DA-47F9686DC584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18075" yWindow="3525" windowWidth="21600" windowHeight="11385" xr2:uid="{CFCFF21E-6815-4865-9DE0-0DADF51387DA}"/>
+    <workbookView xWindow="-38280" yWindow="9270" windowWidth="21600" windowHeight="11385" xr2:uid="{CFCFF21E-6815-4865-9DE0-0DADF51387DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Largest_cities" sheetId="1" r:id="rId1"/>
@@ -8015,8 +8015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C6CE42B-7840-40D4-8D0E-7CFC8CB55E6A}">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8367,7 +8367,7 @@
       <c r="A25" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="7" t="s">
         <v>91</v>
       </c>
       <c r="C25" s="6" t="s">
@@ -8395,7 +8395,7 @@
       <c r="A27" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="7" t="s">
         <v>54</v>
       </c>
       <c r="C27" s="6" t="s">
@@ -8423,7 +8423,7 @@
       <c r="A29" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C29" s="6" t="s">
@@ -8451,7 +8451,7 @@
       <c r="A31" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C31" s="6" t="s">

</xml_diff>

<commit_message>
Data Cleaning, Proper Names
</commit_message>
<xml_diff>
--- a/Data/Largest_Cities.xlsx
+++ b/Data/Largest_Cities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mariko\Documents\GitHub\Capstone-DATS6501\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF46DBFB-A797-41AE-92DA-47F9686DC584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04262DFA-6170-43C1-982A-78AAF666ECF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38280" yWindow="9270" windowWidth="21600" windowHeight="11385" xr2:uid="{CFCFF21E-6815-4865-9DE0-0DADF51387DA}"/>
+    <workbookView xWindow="-11910" yWindow="5010" windowWidth="21600" windowHeight="11385" xr2:uid="{CFCFF21E-6815-4865-9DE0-0DADF51387DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Largest_cities" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="220">
   <si>
     <t> Alabama</t>
   </si>
@@ -740,6 +740,9 @@
   </si>
   <si>
     <t>Northside</t>
+  </si>
+  <si>
+    <t>* Only downloaded a portion - need to implement limits, and a resume function to complete!</t>
   </si>
 </sst>
 </file>
@@ -8013,10 +8016,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C6CE42B-7840-40D4-8D0E-7CFC8CB55E6A}">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8251,7 +8254,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>31</v>
       </c>
@@ -8265,7 +8268,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>74</v>
       </c>
@@ -8279,7 +8282,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>26</v>
       </c>
@@ -8293,7 +8296,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>12</v>
       </c>
@@ -8307,7 +8310,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>35</v>
       </c>
@@ -8321,7 +8324,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>49</v>
       </c>
@@ -8335,7 +8338,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>71</v>
       </c>
@@ -8349,7 +8352,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
         <v>28</v>
       </c>
@@ -8363,7 +8366,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>90</v>
       </c>
@@ -8377,7 +8380,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>33</v>
       </c>
@@ -8391,7 +8394,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>53</v>
       </c>
@@ -8405,7 +8408,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>21</v>
       </c>
@@ -8419,7 +8422,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>55</v>
       </c>
@@ -8433,11 +8436,11 @@
         <v>151</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="9" t="s">
         <v>61</v>
       </c>
       <c r="C30" s="6" t="s">
@@ -8446,8 +8449,19 @@
       <c r="D30" s="6" t="s">
         <v>165</v>
       </c>
+      <c r="E30" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>8</v>
       </c>
@@ -8461,11 +8475,11 @@
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C32" s="6" t="s">
@@ -8479,7 +8493,7 @@
       <c r="A33" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C33" s="6" t="s">
@@ -8493,7 +8507,7 @@
       <c r="A34" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="7" t="s">
         <v>63</v>
       </c>
       <c r="C34" s="6" t="s">

</xml_diff>